<commit_message>
Druhá verze SQL projektu s opravou, instrukce cti v READM, plus oprava XLSX
</commit_message>
<xml_diff>
--- a/SQL_projekt_analýza.xlsx
+++ b/SQL_projekt_analýza.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnatek\Documents\Moje\Python Data akademie\Data akademie SQL\projekt SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFFA6EA-2D4A-4E43-B202-45A36FB76025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1637CF1-E2BC-40B3-9AF0-DAE800939D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B3A8D6F9-AD2C-49B6-8A60-29C2D26CB7CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Analýza dat" sheetId="1" r:id="rId1"/>
-    <sheet name="v_kamil_hnatek_project_sql_payr" sheetId="10" r:id="rId2"/>
-    <sheet name="v_kamil_hnatek_project_sql_czec" sheetId="7" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="9" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="v_kamil_hnatek_project_sql_payr" sheetId="10" state="hidden" r:id="rId2"/>
+    <sheet name="v_kamil_hnatek_project_sql_czec" sheetId="7" state="hidden" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="9" state="hidden" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="2" hidden="1">v_kamil_hnatek_project_sql_czec!$A$1:$D$13</definedName>
@@ -785,7 +785,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -794,36 +794,32 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -850,16 +846,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -869,6 +859,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2083,9 +2082,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Růst HDP v %</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -2218,9 +2214,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Růst mezd v %</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -2353,9 +2346,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:v>Růst cen v %</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -6640,7 +6630,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8304A265-18BD-41D0-87D1-FB2FF5DAAB8D}" name="Odvětví"/>
     <tableColumn id="2" xr3:uid="{10B015B5-02C7-4461-9EE5-EA0AA55DAF5C}" name="Rok"/>
-    <tableColumn id="3" xr3:uid="{50858ECE-0760-4AB6-A62D-9F6840D9A321}" name="Průměrná mzda v CZK" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{50858ECE-0760-4AB6-A62D-9F6840D9A321}" name="Průměrná mzda v CZK" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6657,12 +6647,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2749E68A-CA49-4910-B76D-40D65DCE1A7B}" uniqueName="1" name="Rok" queryTableFieldId="1" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{F2547254-41E9-4304-AA98-5499A3015C41}" uniqueName="3" name="Průměrná mzda" queryTableFieldId="3" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{80F7695B-9949-4043-98D8-49F929C266A2}" uniqueName="5" name="Průměrná cena jídla" queryTableFieldId="5" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{DE286CB4-0D9C-426B-9366-A2FBF12981AD}" uniqueName="2" name="Nárůst mezd v %" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{0A478EFE-D856-40A4-A2DF-81C0215E97E1}" uniqueName="4" name="Nárůst cen v %" queryTableFieldId="4" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{30FADC57-3637-4897-97DB-16828B2D1F0D}" uniqueName="6" name="Rozdíl" queryTableFieldId="8" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{2749E68A-CA49-4910-B76D-40D65DCE1A7B}" uniqueName="1" name="Rok" queryTableFieldId="1" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{F2547254-41E9-4304-AA98-5499A3015C41}" uniqueName="3" name="Průměrná mzda" queryTableFieldId="3" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{80F7695B-9949-4043-98D8-49F929C266A2}" uniqueName="5" name="Průměrná cena jídla" queryTableFieldId="5" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{DE286CB4-0D9C-426B-9366-A2FBF12981AD}" uniqueName="2" name="Nárůst mezd v %" queryTableFieldId="2" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{0A478EFE-D856-40A4-A2DF-81C0215E97E1}" uniqueName="4" name="Nárůst cen v %" queryTableFieldId="4" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{30FADC57-3637-4897-97DB-16828B2D1F0D}" uniqueName="6" name="Rozdíl" queryTableFieldId="8" dataDxfId="11">
       <calculatedColumnFormula>v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst mezd v %]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6676,9 +6666,9 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{29C3476F-3EAF-4F3E-8FC6-CDEF401487BD}" uniqueName="1" name="Rok" queryTableFieldId="1"/>
     <tableColumn id="3" xr3:uid="{A9B7381A-85E9-4670-884F-1187BB262ADF}" uniqueName="3" name="Průměrná mzda" queryTableFieldId="3" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{AC038DEB-00B7-4396-BEC5-AB86EAC0A2B6}" uniqueName="5" name="Průměrná cena jídla" queryTableFieldId="5" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{11D8B11A-8C0C-4075-A1C1-873C72F30412}" uniqueName="2" name="Nárůst mezd v %" queryTableFieldId="2" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{8A0FC39C-1A14-4A75-982D-DA2484EA2A96}" uniqueName="4" name="Nárůst cen v %" queryTableFieldId="4" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{AC038DEB-00B7-4396-BEC5-AB86EAC0A2B6}" uniqueName="5" name="Průměrná cena jídla" queryTableFieldId="5" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{11D8B11A-8C0C-4075-A1C1-873C72F30412}" uniqueName="2" name="Nárůst mezd v %" queryTableFieldId="2" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{8A0FC39C-1A14-4A75-982D-DA2484EA2A96}" uniqueName="4" name="Nárůst cen v %" queryTableFieldId="4" dataDxfId="7"/>
     <tableColumn id="6" xr3:uid="{EA22B2B0-1B4B-4F1D-A3D9-7EF938DB24CA}" uniqueName="6" name="Rozdíl" queryTableFieldId="8" dataDxfId="6">
       <calculatedColumnFormula>v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst mezd v %]]</calculatedColumnFormula>
     </tableColumn>
@@ -6692,9 +6682,9 @@
   <autoFilter ref="A1:D13" xr:uid="{7CF90F13-9629-43C4-B6E1-EADE2D19B9CE}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{8964F626-340C-4A5B-B628-5743EF71D9AF}" uniqueName="1" name="start_year" queryTableFieldId="1"/>
-    <tableColumn id="5" xr3:uid="{78B5CE87-25D0-487D-9782-135DEA31BC12}" uniqueName="5" name="annual_GDP_increase_percent" queryTableFieldId="5" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{FAB0AF59-5558-4361-9FD0-003AD2908CD7}" uniqueName="6" name="annual_payroll_increase_percent" queryTableFieldId="6" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{E5A490C4-2927-49CE-94AB-2B8B95FCC5BB}" uniqueName="7" name="annual_price_increase_percent" queryTableFieldId="7" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{78B5CE87-25D0-487D-9782-135DEA31BC12}" uniqueName="5" name="annual_GDP_increase_percent" queryTableFieldId="5" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{FAB0AF59-5558-4361-9FD0-003AD2908CD7}" uniqueName="6" name="annual_payroll_increase_percent" queryTableFieldId="6" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{E5A490C4-2927-49CE-94AB-2B8B95FCC5BB}" uniqueName="7" name="annual_price_increase_percent" queryTableFieldId="7" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6729,7 +6719,7 @@
   <autoFilter ref="A1:B23" xr:uid="{6FD5D6B0-E929-4D52-95CF-C05DE5F38D32}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1251A8FC-2428-40C3-9B57-4130FE1D3F16}" name="year"/>
-    <tableColumn id="3" xr3:uid="{B353A380-D952-4D54-84F2-80C7DCA1AAA5}" name="average_payroll_value" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{B353A380-D952-4D54-84F2-80C7DCA1AAA5}" name="average_payroll_value" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6741,8 +6731,8 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{ED1315E9-B1BD-4236-AB18-7BB7D9436438}" name="year"/>
     <tableColumn id="2" xr3:uid="{A978F494-1981-40FF-BA45-94281663633E}" name="average_payroll_value"/>
-    <tableColumn id="3" xr3:uid="{D95F15BF-B208-4735-AF22-1CA1D8FB536D}" name="milk_quantity" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{0CB49FCB-449C-4E17-805E-E9D950A9DEDA}" name="bread_quantity" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{D95F15BF-B208-4735-AF22-1CA1D8FB536D}" name="milk_quantity" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{0CB49FCB-449C-4E17-805E-E9D950A9DEDA}" name="bread_quantity" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7069,7 +7059,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7093,13 +7083,13 @@
     <row r="4" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
@@ -7131,7 +7121,7 @@
       <c r="C14">
         <v>2000</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -7142,7 +7132,7 @@
       <c r="C15">
         <v>2020</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -7153,7 +7143,7 @@
       <c r="C16">
         <v>2000</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="9" t="s">
         <v>42</v>
       </c>
     </row>
@@ -7164,7 +7154,7 @@
       <c r="C17">
         <v>2020</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -7175,7 +7165,7 @@
       <c r="C18">
         <v>2000</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -7186,7 +7176,7 @@
       <c r="C19">
         <v>2020</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -7197,7 +7187,7 @@
       <c r="C20">
         <v>2000</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -7208,7 +7198,7 @@
       <c r="C21">
         <v>2020</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="9" t="s">
         <v>49</v>
       </c>
     </row>
@@ -7219,7 +7209,7 @@
       <c r="C22">
         <v>2000</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -7230,7 +7220,7 @@
       <c r="C23">
         <v>2020</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="9" t="s">
         <v>70</v>
       </c>
     </row>
@@ -7241,7 +7231,7 @@
       <c r="C24">
         <v>2000</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="9" t="s">
         <v>72</v>
       </c>
     </row>
@@ -7252,7 +7242,7 @@
       <c r="C25">
         <v>2020</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="9" t="s">
         <v>73</v>
       </c>
     </row>
@@ -7263,7 +7253,7 @@
       <c r="C26">
         <v>2000</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="9" t="s">
         <v>75</v>
       </c>
     </row>
@@ -7274,7 +7264,7 @@
       <c r="C27">
         <v>2020</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="9" t="s">
         <v>76</v>
       </c>
     </row>
@@ -7285,7 +7275,7 @@
       <c r="C28">
         <v>2000</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="9" t="s">
         <v>77</v>
       </c>
     </row>
@@ -7296,7 +7286,7 @@
       <c r="C29">
         <v>2020</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="9" t="s">
         <v>97</v>
       </c>
     </row>
@@ -7307,7 +7297,7 @@
       <c r="C30">
         <v>2000</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="9" t="s">
         <v>99</v>
       </c>
     </row>
@@ -7318,7 +7308,7 @@
       <c r="C31">
         <v>2020</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="9" t="s">
         <v>100</v>
       </c>
     </row>
@@ -7329,7 +7319,7 @@
       <c r="C32">
         <v>2000</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="9" t="s">
         <v>102</v>
       </c>
     </row>
@@ -7340,7 +7330,7 @@
       <c r="C33">
         <v>2020</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="9" t="s">
         <v>103</v>
       </c>
     </row>
@@ -7351,7 +7341,7 @@
       <c r="C34">
         <v>2000</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="9" t="s">
         <v>104</v>
       </c>
     </row>
@@ -7362,7 +7352,7 @@
       <c r="C35">
         <v>2020</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="9" t="s">
         <v>124</v>
       </c>
     </row>
@@ -7373,7 +7363,7 @@
       <c r="C36">
         <v>2000</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="9" t="s">
         <v>126</v>
       </c>
     </row>
@@ -7384,7 +7374,7 @@
       <c r="C37">
         <v>2020</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="9" t="s">
         <v>127</v>
       </c>
     </row>
@@ -7395,7 +7385,7 @@
       <c r="C38">
         <v>2000</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="9" t="s">
         <v>129</v>
       </c>
     </row>
@@ -7406,7 +7396,7 @@
       <c r="C39">
         <v>2020</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="9" t="s">
         <v>130</v>
       </c>
     </row>
@@ -7417,7 +7407,7 @@
       <c r="C40">
         <v>2000</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="9" t="s">
         <v>131</v>
       </c>
     </row>
@@ -7428,7 +7418,7 @@
       <c r="C41">
         <v>2020</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="9" t="s">
         <v>151</v>
       </c>
     </row>
@@ -7439,7 +7429,7 @@
       <c r="C42">
         <v>2000</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="9" t="s">
         <v>153</v>
       </c>
     </row>
@@ -7450,7 +7440,7 @@
       <c r="C43">
         <v>2020</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="9" t="s">
         <v>154</v>
       </c>
     </row>
@@ -7461,7 +7451,7 @@
       <c r="C44">
         <v>2000</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="9" t="s">
         <v>156</v>
       </c>
     </row>
@@ -7472,7 +7462,7 @@
       <c r="C45">
         <v>2020</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="9" t="s">
         <v>157</v>
       </c>
     </row>
@@ -7483,7 +7473,7 @@
       <c r="C46">
         <v>2000</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -7494,7 +7484,7 @@
       <c r="C47">
         <v>2020</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="9" t="s">
         <v>160</v>
       </c>
     </row>
@@ -7505,7 +7495,7 @@
       <c r="C48">
         <v>2000</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="9" t="s">
         <v>161</v>
       </c>
     </row>
@@ -7516,7 +7506,7 @@
       <c r="C49">
         <v>2020</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="9" t="s">
         <v>162</v>
       </c>
     </row>
@@ -7527,7 +7517,7 @@
       <c r="C50">
         <v>2000</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="9" t="s">
         <v>164</v>
       </c>
     </row>
@@ -7538,7 +7528,7 @@
       <c r="C51">
         <v>2020</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="9" t="s">
         <v>165</v>
       </c>
     </row>
@@ -7548,17 +7538,17 @@
       </c>
     </row>
     <row r="54" spans="2:10" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="11"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="12"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B56" s="6" t="s">
@@ -7578,16 +7568,16 @@
       </c>
     </row>
     <row r="76" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="11" t="s">
+      <c r="B76" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="11"/>
-      <c r="I76" s="11"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B78" s="6" t="s">
@@ -7602,16 +7592,16 @@
       </c>
     </row>
     <row r="82" spans="2:22" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B82" s="11" t="s">
+      <c r="B82" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="C82" s="11"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11"/>
-      <c r="I82" s="11"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+      <c r="I82" s="12"/>
     </row>
     <row r="84" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B84" s="6" t="s">
@@ -7647,253 +7637,253 @@
       </c>
     </row>
     <row r="89" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B89" s="9">
+      <c r="B89" s="8">
         <v>2007</v>
       </c>
-      <c r="C89" s="10" t="s">
+      <c r="C89" t="s">
         <v>3</v>
       </c>
-      <c r="D89" s="10" t="s">
+      <c r="D89" t="s">
         <v>176</v>
       </c>
-      <c r="E89" s="10">
+      <c r="E89">
         <v>6.84</v>
       </c>
-      <c r="F89" s="10">
+      <c r="F89">
         <v>6.76</v>
       </c>
-      <c r="G89" s="13">
+      <c r="G89" s="10">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst mezd v %]]</f>
         <v>-8.0000000000000071E-2</v>
       </c>
     </row>
     <row r="90" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B90" s="9">
+      <c r="B90" s="8">
         <v>2008</v>
       </c>
-      <c r="C90" s="10" t="s">
+      <c r="C90" t="s">
         <v>4</v>
       </c>
-      <c r="D90" s="10" t="s">
+      <c r="D90" t="s">
         <v>177</v>
       </c>
-      <c r="E90" s="10">
+      <c r="E90">
         <v>7.87</v>
       </c>
-      <c r="F90" s="10">
+      <c r="F90">
         <v>6.18</v>
       </c>
-      <c r="G90" s="13">
+      <c r="G90" s="10">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst mezd v %]]</f>
         <v>-1.6900000000000004</v>
       </c>
     </row>
     <row r="91" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B91" s="9">
+      <c r="B91" s="8">
         <v>2009</v>
       </c>
-      <c r="C91" s="10" t="s">
+      <c r="C91" t="s">
         <v>5</v>
       </c>
-      <c r="D91" s="10" t="s">
+      <c r="D91" t="s">
         <v>178</v>
       </c>
-      <c r="E91" s="10">
+      <c r="E91">
         <v>3.16</v>
       </c>
-      <c r="F91" s="10">
+      <c r="F91">
         <v>-6.41</v>
       </c>
-      <c r="G91" s="13">
+      <c r="G91" s="10">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst mezd v %]]</f>
         <v>-9.57</v>
       </c>
     </row>
     <row r="92" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B92" s="9">
+      <c r="B92" s="8">
         <v>2010</v>
       </c>
-      <c r="C92" s="10" t="s">
+      <c r="C92" t="s">
         <v>6</v>
       </c>
-      <c r="D92" s="10" t="s">
+      <c r="D92" t="s">
         <v>179</v>
       </c>
-      <c r="E92" s="10">
+      <c r="E92">
         <v>1.95</v>
       </c>
-      <c r="F92" s="10">
+      <c r="F92">
         <v>1.95</v>
       </c>
-      <c r="G92" s="13">
+      <c r="G92" s="10">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst mezd v %]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B93" s="9">
+      <c r="B93" s="8">
         <v>2011</v>
       </c>
-      <c r="C93" s="10" t="s">
+      <c r="C93" t="s">
         <v>7</v>
       </c>
-      <c r="D93" s="10" t="s">
+      <c r="D93" t="s">
         <v>180</v>
       </c>
-      <c r="E93" s="10">
+      <c r="E93">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F93" s="10">
+      <c r="F93">
         <v>3.35</v>
       </c>
-      <c r="G93" s="13">
+      <c r="G93" s="10">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst mezd v %]]</f>
         <v>1.0500000000000003</v>
       </c>
     </row>
     <row r="94" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B94" s="9">
+      <c r="B94" s="8">
         <v>2012</v>
       </c>
-      <c r="C94" s="10" t="s">
+      <c r="C94" t="s">
         <v>8</v>
       </c>
-      <c r="D94" s="10" t="s">
+      <c r="D94" t="s">
         <v>181</v>
       </c>
-      <c r="E94" s="10">
+      <c r="E94">
         <v>3.03</v>
       </c>
-      <c r="F94" s="10">
+      <c r="F94">
         <v>6.73</v>
       </c>
-      <c r="G94" s="13">
+      <c r="G94" s="10">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst mezd v %]]</f>
         <v>3.7000000000000006</v>
       </c>
     </row>
     <row r="95" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B95" s="9">
+      <c r="B95" s="8">
         <v>2013</v>
       </c>
-      <c r="C95" s="10" t="s">
+      <c r="C95" t="s">
         <v>9</v>
       </c>
-      <c r="D95" s="10" t="s">
+      <c r="D95" t="s">
         <v>182</v>
       </c>
-      <c r="E95" s="10">
+      <c r="E95">
         <v>-1.56</v>
       </c>
-      <c r="F95" s="10">
+      <c r="F95">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G95" s="13">
+      <c r="G95" s="10">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst mezd v %]]</f>
         <v>6.66</v>
       </c>
     </row>
     <row r="96" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B96" s="9">
+      <c r="B96" s="8">
         <v>2014</v>
       </c>
-      <c r="C96" s="10" t="s">
+      <c r="C96" t="s">
         <v>10</v>
       </c>
-      <c r="D96" s="10" t="s">
+      <c r="D96" t="s">
         <v>183</v>
       </c>
-      <c r="E96" s="10">
+      <c r="E96">
         <v>2.56</v>
       </c>
-      <c r="F96" s="10">
+      <c r="F96">
         <v>0.74</v>
       </c>
-      <c r="G96" s="13">
+      <c r="G96" s="10">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst mezd v %]]</f>
         <v>-1.82</v>
       </c>
     </row>
     <row r="97" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B97" s="9">
+      <c r="B97" s="8">
         <v>2015</v>
       </c>
-      <c r="C97" s="10" t="s">
+      <c r="C97" t="s">
         <v>11</v>
       </c>
-      <c r="D97" s="10" t="s">
+      <c r="D97" t="s">
         <v>184</v>
       </c>
-      <c r="E97" s="10">
+      <c r="E97">
         <v>2.5099999999999998</v>
       </c>
-      <c r="F97" s="10">
+      <c r="F97">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="G97" s="13">
+      <c r="G97" s="10">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst mezd v %]]</f>
         <v>-3.0599999999999996</v>
       </c>
     </row>
     <row r="98" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B98" s="9">
+      <c r="B98" s="8">
         <v>2016</v>
       </c>
-      <c r="C98" s="10" t="s">
+      <c r="C98" t="s">
         <v>12</v>
       </c>
-      <c r="D98" s="10" t="s">
+      <c r="D98" t="s">
         <v>185</v>
       </c>
-      <c r="E98" s="10">
+      <c r="E98">
         <v>3.65</v>
       </c>
-      <c r="F98" s="10">
+      <c r="F98">
         <v>-1.19</v>
       </c>
-      <c r="G98" s="13">
+      <c r="G98" s="10">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst mezd v %]]</f>
         <v>-4.84</v>
       </c>
     </row>
     <row r="99" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B99" s="9">
+      <c r="B99" s="8">
         <v>2017</v>
       </c>
-      <c r="C99" s="10" t="s">
+      <c r="C99" t="s">
         <v>13</v>
       </c>
-      <c r="D99" s="10" t="s">
+      <c r="D99" t="s">
         <v>186</v>
       </c>
-      <c r="E99" s="10">
+      <c r="E99">
         <v>6.28</v>
       </c>
-      <c r="F99" s="10">
+      <c r="F99">
         <v>9.6300000000000008</v>
       </c>
-      <c r="G99" s="13">
+      <c r="G99" s="10">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst mezd v %]]</f>
         <v>3.3500000000000005</v>
       </c>
     </row>
     <row r="100" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B100" s="9">
+      <c r="B100" s="8">
         <v>2018</v>
       </c>
-      <c r="C100" s="10" t="s">
+      <c r="C100" t="s">
         <v>14</v>
       </c>
-      <c r="D100" s="10" t="s">
+      <c r="D100" t="s">
         <v>187</v>
       </c>
-      <c r="E100" s="10">
+      <c r="E100">
         <v>7.62</v>
       </c>
-      <c r="F100" s="10">
+      <c r="F100">
         <v>2.17</v>
       </c>
-      <c r="G100" s="13">
+      <c r="G100" s="10">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_20241112210315[[#This Row],[Nárůst mezd v %]]</f>
         <v>-5.45</v>
       </c>
@@ -7912,29 +7902,29 @@
       <c r="V104" s="7"/>
     </row>
     <row r="106" spans="2:22" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B106" s="11" t="s">
+      <c r="B106" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C106" s="11"/>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11"/>
-      <c r="F106" s="11"/>
-      <c r="G106" s="11"/>
-      <c r="H106" s="11"/>
-      <c r="I106" s="11"/>
+      <c r="C106" s="12"/>
+      <c r="D106" s="12"/>
+      <c r="E106" s="12"/>
+      <c r="F106" s="12"/>
+      <c r="G106" s="12"/>
+      <c r="H106" s="12"/>
+      <c r="I106" s="12"/>
     </row>
     <row r="124" spans="2:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B124" s="11" t="s">
+      <c r="B124" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C124" s="11"/>
-      <c r="D124" s="11"/>
-      <c r="E124" s="11"/>
-      <c r="F124" s="11"/>
-      <c r="G124" s="11"/>
-      <c r="H124" s="11"/>
-      <c r="I124" s="11"/>
-      <c r="J124" s="11"/>
+      <c r="C124" s="12"/>
+      <c r="D124" s="12"/>
+      <c r="E124" s="12"/>
+      <c r="F124" s="12"/>
+      <c r="G124" s="12"/>
+      <c r="H124" s="12"/>
+      <c r="I124" s="12"/>
+      <c r="J124" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -7997,19 +7987,19 @@
       <c r="A2">
         <v>2007</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" t="s">
         <v>176</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2">
         <v>6.84</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2">
         <v>6.76</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst mezd v %]]</f>
         <v>-8.0000000000000071E-2</v>
       </c>
@@ -8018,19 +8008,19 @@
       <c r="A3">
         <v>2008</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" t="s">
         <v>177</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3">
         <v>7.87</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3">
         <v>6.18</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst mezd v %]]</f>
         <v>-1.6900000000000004</v>
       </c>
@@ -8039,19 +8029,19 @@
       <c r="A4">
         <v>2009</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" t="s">
         <v>178</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4">
         <v>3.16</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4">
         <v>-6.41</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst mezd v %]]</f>
         <v>-9.57</v>
       </c>
@@ -8060,19 +8050,19 @@
       <c r="A5">
         <v>2010</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" t="s">
         <v>179</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5">
         <v>1.95</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5">
         <v>1.95</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst mezd v %]]</f>
         <v>0</v>
       </c>
@@ -8081,19 +8071,19 @@
       <c r="A6">
         <v>2011</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" t="s">
         <v>180</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6">
         <v>3.35</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst mezd v %]]</f>
         <v>1.0500000000000003</v>
       </c>
@@ -8102,19 +8092,19 @@
       <c r="A7">
         <v>2012</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7">
         <v>3.03</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7">
         <v>6.73</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst mezd v %]]</f>
         <v>3.7000000000000006</v>
       </c>
@@ -8123,19 +8113,19 @@
       <c r="A8">
         <v>2013</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" t="s">
         <v>182</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8">
         <v>-1.56</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst mezd v %]]</f>
         <v>6.66</v>
       </c>
@@ -8144,19 +8134,19 @@
       <c r="A9">
         <v>2014</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" t="s">
         <v>183</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9">
         <v>2.56</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9">
         <v>0.74</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst mezd v %]]</f>
         <v>-1.82</v>
       </c>
@@ -8165,19 +8155,19 @@
       <c r="A10">
         <v>2015</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" t="s">
         <v>184</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10">
         <v>2.5099999999999998</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst mezd v %]]</f>
         <v>-3.0599999999999996</v>
       </c>
@@ -8186,19 +8176,19 @@
       <c r="A11">
         <v>2016</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" t="s">
         <v>185</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11">
         <v>3.65</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11">
         <v>-1.19</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst mezd v %]]</f>
         <v>-4.84</v>
       </c>
@@ -8207,19 +8197,19 @@
       <c r="A12">
         <v>2017</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" t="s">
         <v>186</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12">
         <v>6.28</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12">
         <v>9.6300000000000008</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst mezd v %]]</f>
         <v>3.3500000000000005</v>
       </c>
@@ -8228,19 +8218,19 @@
       <c r="A13">
         <v>2018</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" t="s">
         <v>187</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13">
         <v>7.62</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13">
         <v>2.17</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13">
         <f>v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst cen v %]]-v_kamil_hnatek_project_sql_payroll_annual_increase_202411122103[[#This Row],[Nárůst mezd v %]]</f>
         <v>-5.45</v>
       </c>
@@ -8258,7 +8248,7 @@
   <dimension ref="A1:E331"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8959,7 +8949,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9410,7 +9400,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>